<commit_message>
Updates to Pioneer 07 & 08 summary sheets; added Pioneer 09 summary sheet.
</commit_message>
<xml_diff>
--- a/Ship_data/Pioneer/Pioneer-07_AR-08_2016-09-27/Pioneer-07_AR08_Discrete_Summary_2019-06-19_ver_1-01_.xlsx
+++ b/Ship_data/Pioneer/Pioneer-07_AR-08_2016-09-27/Pioneer-07_AR08_Discrete_Summary_2019-06-19_ver_1-01_.xlsx
@@ -49,10 +49,10 @@
     <t xml:space="preserve">Bottom Depth [m]</t>
   </si>
   <si>
-    <t xml:space="preserve">Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Flag</t>
+    <t xml:space="preserve">CTD Filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD File Flag</t>
   </si>
   <si>
     <t xml:space="preserve">Bottle Position</t>
@@ -61,82 +61,82 @@
     <t xml:space="preserve">Niskin Flag</t>
   </si>
   <si>
-    <t xml:space="preserve">Bottle Closure Time [UTC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure, Digiquartz [db]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth [salt water, m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude [deg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude [deg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature [ITS-90, deg C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature 1 Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature, 2 [ITS-90, deg C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature 2 Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity [S/m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity 1 Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity, 2 [S/m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity 2 Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salinity, Practical [PSU]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salinity, Practical, 2 [PSU]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen, SBE 43 [ml/l]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen Saturation, Garcia &amp; Gordon [ml/l]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluorescence [mg/m^3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluorescence Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam Attenuation, WET Labs C-Star [1/m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam Transmission, WET Labs C-Star [%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transmissometer Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH Flag</t>
+    <t xml:space="preserve">CTD Bottle Closure Time [UTC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Pressure, Digiquartz [db]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Pressure Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Depth [salt water, m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Latitude [deg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Longitude [deg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Temperature [ITS-90, deg C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Temperature 1 Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Temperature, 2 [ITS-90, deg C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Temperature 2 Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Conductivity [S/m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Conductivity 1 Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Conductivity, 2 [S/m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Conductivity 2 Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Salinity, Practical [PSU]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Salinity, Practical, 2 [PSU]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Oxygen, SBE 43 [ml/l]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Oxygen Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Oxygen Saturation, Garcia &amp; Gordon [ml/l]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Fluorescence [mg/m^3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Fluorescence Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Beam Attenuation, WET Labs C-Star [1/m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Beam Transmission, WET Labs C-Star [%]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD Transmissometer Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTD pH Flag</t>
   </si>
   <si>
     <t xml:space="preserve">Discrete Oxygen [mL/L]</t>
@@ -1935,11 +1935,11 @@
   <dimension ref="A1:BY171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BY1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5319" ySplit="570" topLeftCell="BN30" activePane="bottomRight" state="split"/>
+      <pane xSplit="5013" ySplit="570" topLeftCell="A30" activePane="bottomRight" state="split"/>
       <selection pane="topLeft" activeCell="BY1" activeCellId="0" sqref="BY1"/>
-      <selection pane="topRight" activeCell="BN1" activeCellId="0" sqref="BN1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="BY30" activeCellId="0" sqref="BY30"/>
-      <selection pane="bottomRight" activeCell="BN39" activeCellId="0" sqref="BN39"/>
+      <selection pane="bottomRight" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1950,38 +1950,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="27.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="25.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="31.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="33.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="27.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="40.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="40.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="39.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="21.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="44.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="27.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="22.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="44.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="43.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="25.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="12.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="23.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="21.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="30.47"/>
@@ -1992,7 +1993,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="35.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="24.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="23.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="22.74"/>
@@ -2023,7 +2024,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="78" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>